<commit_message>
fixed test so far
</commit_message>
<xml_diff>
--- a/tests/Stud1 Solver Simple.xlsx
+++ b/tests/Stud1 Solver Simple.xlsx
@@ -195,7 +195,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -214,6 +214,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -239,7 +243,7 @@
       <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.05078125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.05859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
@@ -319,13 +323,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -338,7 +342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
         <v>1</v>
       </c>
@@ -346,7 +350,17 @@
         <v>11</v>
       </c>
       <c r="C2" s="4" t="n">
+        <v>5952</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>1001</v>
+      </c>
+      <c r="F2" s="5" t="n">
         <v>4951</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">E2+F2</f>
+        <v>5952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>